<commit_message>
Formatting, Conditional Formatting, Filter
</commit_message>
<xml_diff>
--- a/Excel/Data files/Lecture_2.xlsx
+++ b/Excel/Data files/Lecture_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ds_30\Excel\Data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDE2FFE-AFA6-43D0-A7E0-B2E60C220C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F792A0AE-C7FD-4F87-8784-4F8F9A99D645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRIM" sheetId="2" r:id="rId1"/>
@@ -712,63 +712,67 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,10 +811,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1696,10 +1696,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="54"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1707,24 +1707,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -1733,13 +1733,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -1750,19 +1750,19 @@
       <c r="M4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="53" t="s">
+      <c r="N4" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="40"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -1774,21 +1774,21 @@
         <f>TRIM(L5)</f>
         <v>Student 1</v>
       </c>
-      <c r="N5" s="54" t="s">
+      <c r="N5" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
       <c r="Q5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="40"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
       <c r="L6" s="24" t="s">
         <v>40</v>
       </c>
@@ -1796,18 +1796,18 @@
         <f t="shared" ref="M6:M7" si="0">TRIM(L6)</f>
         <v>Student 1</v>
       </c>
-      <c r="N6" s="54" t="s">
+      <c r="N6" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="40"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41"/>
       <c r="L7" s="24" t="s">
         <v>41</v>
       </c>
@@ -1815,47 +1815,47 @@
         <f t="shared" si="0"/>
         <v>Student 1</v>
       </c>
-      <c r="N7" s="54" t="s">
+      <c r="N7" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="40"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
       <c r="M9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="38"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41"/>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="43"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -1866,67 +1866,72 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="C4:G11"/>
     <mergeCell ref="C14:G21"/>
     <mergeCell ref="K1:L1"/>
@@ -1937,11 +1942,6 @@
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1952,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="69" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="59" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1987,24 +1987,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2017,13 +2017,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="57"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -2042,11 +2042,11 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -2064,11 +2064,11 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
       <c r="K6" s="28" t="s">
         <v>43</v>
       </c>
@@ -2083,11 +2083,11 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
       <c r="K7" s="28" t="s">
         <v>44</v>
       </c>
@@ -2102,11 +2102,11 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="58"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
       <c r="K8" s="28" t="s">
         <v>45</v>
       </c>
@@ -2121,11 +2121,11 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
       <c r="K9" s="28" t="s">
         <v>46</v>
       </c>
@@ -2140,19 +2140,19 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -2169,13 +2169,13 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
       <c r="K14" s="22" t="s">
         <v>1</v>
       </c>
@@ -2191,11 +2191,11 @@
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
       <c r="K15" s="28" t="s">
         <v>42</v>
       </c>
@@ -2203,7 +2203,10 @@
         <f>CONCATENATE(K15," has scored ",L5, " in Maths")</f>
         <v>Student 1 has scored 95 in Maths</v>
       </c>
-      <c r="M15" s="28"/>
+      <c r="M15" s="28" t="str">
+        <f>CONCATENATE(K15," has scored ",M5," in Science.")</f>
+        <v>Student 1 has scored 83 in Science.</v>
+      </c>
       <c r="N15" s="28" t="str">
         <f>K15&amp;" has scored "&amp;N5&amp;" in English."</f>
         <v>Student 1 has scored 81 in English.</v>
@@ -2211,11 +2214,11 @@
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
       <c r="K16" s="28" t="s">
         <v>43</v>
       </c>
@@ -2223,18 +2226,21 @@
         <f t="shared" ref="L16:L19" si="0">CONCATENATE(K16," has scored ",L6, " in Maths")</f>
         <v>Student 2 has scored 65 in Maths</v>
       </c>
-      <c r="M16" s="28"/>
+      <c r="M16" s="28" t="str">
+        <f>K16&amp;" has scored "&amp;M6&amp;" in Science."</f>
+        <v>Student 2 has scored 53 in Science.</v>
+      </c>
       <c r="N16" s="28" t="str">
         <f t="shared" ref="N16:N19" si="1">K16&amp;" has scored "&amp;N6&amp;" in English."</f>
         <v>Student 2 has scored 75 in English.</v>
       </c>
     </row>
     <row r="17" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
       <c r="K17" s="28" t="s">
         <v>44</v>
       </c>
@@ -2242,18 +2248,21 @@
         <f t="shared" si="0"/>
         <v>Student 3 has scored 85 in Maths</v>
       </c>
-      <c r="M17" s="28"/>
+      <c r="M17" s="28" t="str">
+        <f t="shared" ref="M17:M19" si="2">K17&amp;" has scored "&amp;M7&amp;" in Science."</f>
+        <v>Student 3 has scored 80 in Science.</v>
+      </c>
       <c r="N17" s="28" t="str">
         <f t="shared" si="1"/>
         <v>Student 3 has scored 90 in English.</v>
       </c>
     </row>
     <row r="18" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
       <c r="K18" s="28" t="s">
         <v>45</v>
       </c>
@@ -2261,18 +2270,21 @@
         <f t="shared" si="0"/>
         <v>Student 4 has scored 99 in Maths</v>
       </c>
-      <c r="M18" s="28"/>
+      <c r="M18" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v>Student 4 has scored 99 in Science.</v>
+      </c>
       <c r="N18" s="28" t="str">
         <f t="shared" si="1"/>
         <v>Student 4 has scored 85 in English.</v>
       </c>
     </row>
     <row r="19" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
       <c r="K19" s="28" t="s">
         <v>46</v>
       </c>
@@ -2280,25 +2292,28 @@
         <f t="shared" si="0"/>
         <v>Student 5 has scored 45 in Maths</v>
       </c>
-      <c r="M19" s="28"/>
+      <c r="M19" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v>Student 5 has scored 60 in Science.</v>
+      </c>
       <c r="N19" s="28" t="str">
         <f t="shared" si="1"/>
         <v>Student 5 has scored 55 in English.</v>
       </c>
     </row>
     <row r="20" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="3:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2358,23 +2373,23 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="34"/>
+      <c r="L1" s="54"/>
       <c r="M1" s="15"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
       <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2383,13 +2398,13 @@
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="57"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -2397,117 +2412,117 @@
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="60"/>
-      <c r="K6" s="53" t="s">
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
+      <c r="K6" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53" t="s">
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53" t="s">
+      <c r="O6" s="55"/>
+      <c r="P6" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60"/>
-      <c r="K7" s="64" t="s">
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+      <c r="K7" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64" t="str">
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="66" t="str">
         <f>SUBSTITUTE(K7,"b","d")</f>
         <v>Student</v>
       </c>
-      <c r="O7" s="64"/>
-      <c r="P7" s="54" t="s">
+      <c r="O7" s="66"/>
+      <c r="P7" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="58"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
-      <c r="K8" s="64" t="s">
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
+      <c r="K8" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64" t="str">
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66" t="str">
         <f>SUBSTITUTE(K8,"38","65")</f>
         <v>Student 1 scored 65 marks in Science</v>
       </c>
-      <c r="O8" s="64"/>
-      <c r="P8" s="54" t="s">
+      <c r="O8" s="66"/>
+      <c r="P8" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
-      <c r="K9" s="64" t="s">
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+      <c r="K9" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64" t="str">
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66" t="str">
         <f>SUBSTITUTE(K9,"Science","english")</f>
         <v>Student 1 scored 85 marks in english</v>
       </c>
-      <c r="O9" s="64"/>
-      <c r="P9" s="54" t="s">
+      <c r="O9" s="66"/>
+      <c r="P9" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="54"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -2518,67 +2533,72 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:R9"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
@@ -2595,11 +2615,6 @@
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="P7:R7"/>
     <mergeCell ref="K8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2645,23 +2660,23 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
       <c r="O1" s="15"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
       <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2670,13 +2685,13 @@
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="57"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -2693,11 +2708,11 @@
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -2715,11 +2730,11 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
       <c r="L6" s="27" t="s">
         <v>43</v>
       </c>
@@ -2733,11 +2748,11 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
       <c r="L7" s="27" t="s">
         <v>44</v>
       </c>
@@ -2755,11 +2770,11 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="58"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
       <c r="L8" s="27" t="s">
         <v>45</v>
       </c>
@@ -2773,11 +2788,11 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
       <c r="L9" s="27" t="s">
         <v>46</v>
       </c>
@@ -2791,19 +2806,19 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -2814,64 +2829,64 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2930,24 +2945,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2956,13 +2971,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="14"/>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="57"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -2976,11 +2991,11 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -2988,150 +3003,150 @@
       <c r="L5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="67">
+      <c r="M5" s="35">
         <f>LEN(L5)</f>
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
       <c r="L6" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="M6" s="67">
+      <c r="M6" s="35">
         <f t="shared" ref="M6:M9" si="0">LEN(L6)</f>
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
       <c r="L7" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="M7" s="67">
+      <c r="M7" s="35">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="58"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
       <c r="L8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="67">
+      <c r="M8" s="35">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
       <c r="L9" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="M9" s="67">
+      <c r="M9" s="35">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
       <c r="C12" s="12"/>
-      <c r="L12" s="66"/>
+      <c r="L12" s="34"/>
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C13" s="13"/>
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="3:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
     </row>
     <row r="22" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K22" s="26"/>
@@ -3177,7 +3192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -3213,24 +3228,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -3239,24 +3254,24 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="57"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -3274,11 +3289,11 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
       <c r="L6" s="33" t="s">
         <v>56</v>
       </c>
@@ -3296,11 +3311,11 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
       <c r="L7" s="32" t="s">
         <v>57</v>
       </c>
@@ -3318,11 +3333,11 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="58"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
       <c r="L8" s="32" t="s">
         <v>58</v>
       </c>
@@ -3340,11 +3355,11 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
       <c r="L9" s="32" t="s">
         <v>59</v>
       </c>
@@ -3362,11 +3377,11 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
       <c r="L10" s="32" t="s">
         <v>60</v>
       </c>
@@ -3385,11 +3400,11 @@
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
       <c r="L11" s="32" t="s">
         <v>61</v>
       </c>
@@ -3415,64 +3430,64 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="3:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
       <c r="M21" s="21"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Textual Functions and logicals
</commit_message>
<xml_diff>
--- a/Excel/Data files/Lecture_2.xlsx
+++ b/Excel/Data files/Lecture_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ds_30\Excel\Data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FE0C4F-7DC5-4E2A-9E4C-2C5AE643734A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AF28DA-AA35-4478-836E-BDAB72CE77FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRIM" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>Example</t>
   </si>
@@ -96,15 +96,6 @@
   </si>
   <si>
     <t>String</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =TRIM(L16)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =TRIM(L17)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =TRIM(L18)</t>
   </si>
   <si>
     <t>CONCATENATE</t>
@@ -135,9 +126,6 @@
  =LOWER(Text)</t>
   </si>
   <si>
-    <t xml:space="preserve"> =SUBSTITUTE(K9,"Science","English ")</t>
-  </si>
-  <si>
     <t xml:space="preserve"> =LEN(Text)</t>
   </si>
   <si>
@@ -202,12 +190,6 @@
   </si>
   <si>
     <t>Student 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =SUBSTITUTE(K7,"b","d")</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =SUBSTITUTE(K8,"38","95 ")</t>
   </si>
   <si>
     <r>
@@ -293,31 +275,6 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>abcde</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>43</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2018</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -350,6 +307,34 @@
   <si>
     <t>Add A space before = to get result like =TRIM(L16)</t>
   </si>
+  <si>
+    <t xml:space="preserve"> =TRIM(L5)</t>
+  </si>
+  <si>
+    <r>
+      <t>2018</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>abcde</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>43</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -358,7 +343,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +471,13 @@
     <font>
       <sz val="12"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -716,6 +708,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -769,9 +764,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1672,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5:M7"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1696,10 +1688,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="54"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1707,24 +1699,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -1733,13 +1725,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -1758,41 +1750,37 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="41"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
       <c r="K5" s="3"/>
       <c r="L5" s="24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M5" s="24"/>
-      <c r="N5" s="56" t="s">
-        <v>14</v>
-      </c>
+      <c r="N5" s="56"/>
       <c r="O5" s="56"/>
       <c r="P5" s="56"/>
       <c r="Q5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="39"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42"/>
       <c r="L6" s="24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M6" s="24"/>
-      <c r="N6" s="56" t="s">
-        <v>15</v>
-      </c>
+      <c r="N6" s="56"/>
       <c r="O6" s="56"/>
       <c r="P6" s="56"/>
       <c r="Q6">
@@ -1800,56 +1788,57 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="41"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="42"/>
       <c r="L7" s="24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="56" t="s">
-        <v>16</v>
-      </c>
+      <c r="N7" s="56"/>
       <c r="O7" s="56"/>
       <c r="P7" s="56"/>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="41"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
       <c r="M9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="39"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="45"/>
+      <c r="L11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -1860,72 +1849,67 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="C4:G11"/>
     <mergeCell ref="C14:G21"/>
     <mergeCell ref="K1:L1"/>
@@ -1936,6 +1920,11 @@
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1946,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F1" zoomScale="78" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16:N18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="78" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1971,7 +1960,7 @@
     <row r="1" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1981,24 +1970,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2012,7 +2001,7 @@
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
       <c r="C4" s="57" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="58"/>
       <c r="E4" s="58"/>
@@ -2045,7 +2034,7 @@
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
       <c r="K5" s="28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="L5" s="28">
         <v>95</v>
@@ -2064,7 +2053,7 @@
       <c r="F6" s="61"/>
       <c r="G6" s="62"/>
       <c r="K6" s="28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L6" s="28">
         <v>65</v>
@@ -2083,7 +2072,7 @@
       <c r="F7" s="61"/>
       <c r="G7" s="62"/>
       <c r="K7" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L7" s="28">
         <v>85</v>
@@ -2102,7 +2091,7 @@
       <c r="F8" s="61"/>
       <c r="G8" s="62"/>
       <c r="K8" s="28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L8" s="28">
         <v>99</v>
@@ -2121,7 +2110,7 @@
       <c r="F9" s="61"/>
       <c r="G9" s="62"/>
       <c r="K9" s="28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L9" s="28">
         <v>45</v>
@@ -2155,21 +2144,21 @@
     <row r="13" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C13" s="13"/>
       <c r="L13" s="29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N13" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
+      <c r="C14" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
       <c r="K14" s="22" t="s">
         <v>1</v>
       </c>
@@ -2185,90 +2174,90 @@
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
       <c r="K15" s="28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="L15" s="28" t="str">
         <f>CONCATENATE(K15," has scored ",L5," in Maths.")</f>
         <v>Student 1 has scored 95 in Maths.</v>
       </c>
       <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+      <c r="N15" s="28" t="str">
+        <f>K15&amp;" has scored "&amp;N5&amp;" in English."</f>
+        <v>Student 1 has scored 81 in English.</v>
+      </c>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
       <c r="K16" s="28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
     </row>
     <row r="17" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
       <c r="K17" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
       <c r="N17" s="28"/>
     </row>
     <row r="18" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
       <c r="K18" s="28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
     </row>
     <row r="19" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
       <c r="K19" s="28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
-      <c r="N19" s="28" t="str">
-        <f t="shared" ref="N16:N19" si="0">K19&amp;" has scored "&amp;N9&amp;" in English."</f>
-        <v>Student 5 has scored 55 in English.</v>
-      </c>
+      <c r="N19" s="28"/>
     </row>
     <row r="20" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="3:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2292,8 +2281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="N3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7:O8"/>
+    <sheetView showGridLines="0" topLeftCell="F3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8:O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2328,23 +2317,23 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="54"/>
+      <c r="L1" s="36"/>
       <c r="M1" s="15"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
       <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2405,15 +2394,16 @@
       <c r="F7" s="61"/>
       <c r="G7" s="62"/>
       <c r="K7" s="66" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L7" s="66"/>
       <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
+      <c r="N7" s="66" t="str">
+        <f>SUBSTITUTE(K7,"b","d")</f>
+        <v>Student</v>
+      </c>
       <c r="O7" s="66"/>
-      <c r="P7" s="56" t="s">
-        <v>47</v>
-      </c>
+      <c r="P7" s="56"/>
       <c r="Q7" s="56"/>
       <c r="R7" s="56"/>
     </row>
@@ -2424,15 +2414,13 @@
       <c r="F8" s="61"/>
       <c r="G8" s="62"/>
       <c r="K8" s="66" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L8" s="66"/>
       <c r="M8" s="66"/>
       <c r="N8" s="66"/>
       <c r="O8" s="66"/>
-      <c r="P8" s="56" t="s">
-        <v>48</v>
-      </c>
+      <c r="P8" s="56"/>
       <c r="Q8" s="56"/>
       <c r="R8" s="56"/>
     </row>
@@ -2443,15 +2431,13 @@
       <c r="F9" s="61"/>
       <c r="G9" s="62"/>
       <c r="K9" s="66" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="L9" s="66"/>
       <c r="M9" s="66"/>
       <c r="N9" s="66"/>
       <c r="O9" s="66"/>
-      <c r="P9" s="56" t="s">
-        <v>25</v>
-      </c>
+      <c r="P9" s="56"/>
       <c r="Q9" s="56"/>
       <c r="R9" s="56"/>
     </row>
@@ -2479,72 +2465,67 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:R9"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
@@ -2561,6 +2542,11 @@
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="P7:R7"/>
     <mergeCell ref="K8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2596,7 +2582,7 @@
     <row r="1" spans="1:26" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2606,23 +2592,23 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="15"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
       <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2632,7 +2618,7 @@
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
       <c r="C4" s="57" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" s="58"/>
       <c r="E4" s="58"/>
@@ -2646,10 +2632,10 @@
         <v>1</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="N4" s="25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2664,7 +2650,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="3"/>
       <c r="L5" s="27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M5" s="27"/>
       <c r="N5" s="27"/>
@@ -2676,7 +2662,7 @@
       <c r="F6" s="61"/>
       <c r="G6" s="62"/>
       <c r="L6" s="27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M6" s="27"/>
       <c r="N6" s="27"/>
@@ -2688,7 +2674,7 @@
       <c r="F7" s="61"/>
       <c r="G7" s="62"/>
       <c r="L7" s="27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
@@ -2704,7 +2690,7 @@
       <c r="F8" s="61"/>
       <c r="G8" s="62"/>
       <c r="L8" s="27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
@@ -2716,7 +2702,7 @@
       <c r="F9" s="61"/>
       <c r="G9" s="62"/>
       <c r="L9" s="27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
@@ -2745,64 +2731,64 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
+      <c r="C14" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2825,8 +2811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5:M9"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2851,7 +2837,7 @@
     <row r="1" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2861,24 +2847,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2888,7 +2874,7 @@
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="14"/>
       <c r="C4" s="57" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" s="58"/>
       <c r="E4" s="58"/>
@@ -2902,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2917,7 +2903,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="3"/>
       <c r="L5" s="27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M5" s="35"/>
     </row>
@@ -2928,7 +2914,7 @@
       <c r="F6" s="61"/>
       <c r="G6" s="62"/>
       <c r="L6" s="27" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="M6" s="35"/>
     </row>
@@ -2939,7 +2925,7 @@
       <c r="F7" s="61"/>
       <c r="G7" s="62"/>
       <c r="L7" s="27" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="M7" s="35"/>
     </row>
@@ -2950,7 +2936,7 @@
       <c r="F8" s="61"/>
       <c r="G8" s="62"/>
       <c r="L8" s="27" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="M8" s="35"/>
     </row>
@@ -2961,7 +2947,7 @@
       <c r="F9" s="61"/>
       <c r="G9" s="62"/>
       <c r="L9" s="27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="M9" s="35"/>
     </row>
@@ -2990,64 +2976,64 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
+      <c r="C14" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
     </row>
     <row r="17" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
     </row>
     <row r="18" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
     </row>
     <row r="19" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
     </row>
     <row r="20" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="3:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
     </row>
     <row r="22" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K22" s="26"/>
@@ -3093,8 +3079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView showGridLines="0" zoomScale="62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3119,7 +3105,7 @@
     <row r="1" spans="1:27" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3129,24 +3115,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -3156,7 +3142,7 @@
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
       <c r="C4" s="67" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" s="58"/>
       <c r="E4" s="58"/>
@@ -3177,16 +3163,16 @@
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
       <c r="L5" s="31" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M5" s="31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="O5" s="31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3196,7 +3182,7 @@
       <c r="F6" s="61"/>
       <c r="G6" s="62"/>
       <c r="L6" s="33" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
@@ -3209,7 +3195,7 @@
       <c r="F7" s="61"/>
       <c r="G7" s="62"/>
       <c r="L7" s="32" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="M7" s="32"/>
       <c r="N7" s="32"/>
@@ -3222,7 +3208,7 @@
       <c r="F8" s="61"/>
       <c r="G8" s="62"/>
       <c r="L8" s="32" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="M8" s="32"/>
       <c r="N8" s="32"/>
@@ -3235,7 +3221,7 @@
       <c r="F9" s="61"/>
       <c r="G9" s="62"/>
       <c r="L9" s="32" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="M9" s="32"/>
       <c r="N9" s="32"/>
@@ -3248,7 +3234,7 @@
       <c r="F10" s="61"/>
       <c r="G10" s="62"/>
       <c r="L10" s="32" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="M10" s="32"/>
       <c r="N10" s="32"/>
@@ -3262,7 +3248,7 @@
       <c r="F11" s="64"/>
       <c r="G11" s="65"/>
       <c r="L11" s="32" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="M11" s="32"/>
       <c r="N11" s="32"/>
@@ -3277,64 +3263,64 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
+      <c r="C14" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
     </row>
     <row r="17" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="50"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
     </row>
     <row r="18" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
     </row>
     <row r="19" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
     </row>
     <row r="20" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="3:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
       <c r="M21" s="21"/>
     </row>
   </sheetData>

</xml_diff>